<commit_message>
Fix typo in readme
</commit_message>
<xml_diff>
--- a/base_iepd/documentation/superhero-mapping.xlsx
+++ b/base_iepd/documentation/superhero-mapping.xlsx
@@ -157,7 +157,7 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -222,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -231,38 +231,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -291,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -300,15 +272,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,19 +288,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -336,15 +296,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -455,12 +411,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.83"/>
   </cols>
@@ -500,7 +456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="56" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="55.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -531,7 +487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -566,23 +522,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+    <row r="4" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -597,27 +553,27 @@
       <c r="J4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+    <row r="5" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -632,7 +588,7 @@
       <c r="J5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="9" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>